<commit_message>
added getting text pipeline
</commit_message>
<xml_diff>
--- a/process_text/data.xlsx
+++ b/process_text/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runze\OneDrive\Desktop\DaisyHacks2020\process_text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_F25DC773A252ABDACC10488FC19C7E2C5ADE58E9" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A49C37BA-6BFC-4051-B6D6-69006DBC5276}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_F25DC773A252ABDACC10488FC19C7E2C5ADE58E9" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{13A959AF-C44E-420F-8581-48815748CA2B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,11 +30,19 @@
     <t>text</t>
   </si>
   <si>
-    <t>$4 499 /ib.
-SAVE $10/Ib.
+    <t>HEALTHY REWARDS
+OFFER WITH CARD
+$1499/lb. 2
+SAVE $10/lb.
 Fresh, Wild
+NON-GMO
+FRESH
 Sockeye
-Salmon Fillets</t>
+Salmon Fillets
+100% Traceable and Sustainably Sourced, All Earth Fare
+Salmon is non-GMO, Superior Flavor, Great Source of
+Omega-3 Fatty Acids, Product of the USA (Alaska)
+Discount Taken at Register</t>
   </si>
 </sst>
 </file>
@@ -371,7 +379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>